<commit_message>
Supervisión Remoto y Central
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="sRemoto" sheetId="5" r:id="rId1"/>
     <sheet name="ICCP" sheetId="2" r:id="rId2"/>
     <sheet name="AGC" sheetId="3" r:id="rId3"/>
     <sheet name="SISTEMA CENTRAL" sheetId="4" r:id="rId4"/>
+    <sheet name="COLORES" sheetId="6" r:id="rId5"/>
+    <sheet name="TRADUCCION" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="382">
   <si>
     <t>Tag</t>
   </si>
@@ -1143,13 +1145,43 @@
   </si>
   <si>
     <t>MOLINO AGC</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>DISPONIBLE</t>
+  </si>
+  <si>
+    <t>SUSTITUCION</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Operable</t>
+  </si>
+  <si>
+    <t>Inoperable</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Unavailable</t>
+  </si>
+  <si>
+    <t>#b33c00</t>
+  </si>
+  <si>
+    <t>#2bc353</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1163,8 +1195,23 @@
       <name val="Courier New"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1174,6 +1221,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB33C00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2BC253"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1191,7 +1250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
@@ -1202,6 +1261,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,6 +1272,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF2BC253"/>
+      <color rgb="FFB33C00"/>
+      <color rgb="FF00E673"/>
+      <color rgb="FF00FF55"/>
+      <color rgb="FF6EA92D"/>
+      <color rgb="FFDE2A00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1486,7 +1559,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,35 +1577,35 @@
     <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5921,7 +5994,7 @@
   <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5938,32 +6011,32 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>318</v>
       </c>
     </row>
@@ -6060,7 +6133,7 @@
         <v>159</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>327</v>
@@ -6104,7 +6177,7 @@
         <v>159</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>331</v>
@@ -6126,7 +6199,7 @@
         <v>159</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>333</v>
@@ -6170,7 +6243,7 @@
         <v>159</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>337</v>
@@ -6192,7 +6265,7 @@
         <v>159</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>339</v>
@@ -6870,8 +6943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6885,23 +6958,23 @@
     <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>367</v>
       </c>
     </row>
@@ -7346,7 +7419,7 @@
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7361,23 +7434,23 @@
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:7" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>318</v>
       </c>
     </row>
@@ -7457,4 +7530,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Supervisión Remoto y Central corrección colores
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -541,12 +541,6 @@
     <t>UTR_TEST_LAB_RP5.SV</t>
   </si>
   <si>
-    <t>C_CALOPE_DNP.SV</t>
-  </si>
-  <si>
-    <t>S_DOMING_RP5.SV</t>
-  </si>
-  <si>
     <t>TEST_LAB_DNP.SV</t>
   </si>
   <si>
@@ -766,9 +760,6 @@
     <t>CUENCA 1</t>
   </si>
   <si>
-    <t>CUENCA  (BAHIAS YANACOCHA GUALACEO)</t>
-  </si>
-  <si>
     <t>CUENCA</t>
   </si>
   <si>
@@ -814,12 +805,6 @@
     <t>LIMON</t>
   </si>
   <si>
-    <t>LOJA _1</t>
-  </si>
-  <si>
-    <t>LOJA_2</t>
-  </si>
-  <si>
     <t>LOJA</t>
   </si>
   <si>
@@ -862,12 +847,6 @@
     <t>POLICENTRO</t>
   </si>
   <si>
-    <t>POMASQUI_A</t>
-  </si>
-  <si>
-    <t>POMASQUI_B</t>
-  </si>
-  <si>
     <t>PORTOVIEJO</t>
   </si>
   <si>
@@ -883,15 +862,6 @@
     <t>RIOBAMBA</t>
   </si>
   <si>
-    <t>SANTO DOMINGO_A</t>
-  </si>
-  <si>
-    <t>SANTO DOMINGO_B</t>
-  </si>
-  <si>
-    <t>SANTO DOMINGO_C</t>
-  </si>
-  <si>
     <t>SANTA ELENA (BAHIA C SANTA ELENA 3)</t>
   </si>
   <si>
@@ -958,21 +928,12 @@
     <t>YANACOCHA</t>
   </si>
   <si>
-    <t>C_GENEROCA</t>
-  </si>
-  <si>
     <t>D_PERIPA</t>
   </si>
   <si>
     <t>CENTRAL ELECTROQUIL</t>
   </si>
   <si>
-    <t>C_GASGREEN</t>
-  </si>
-  <si>
-    <t>C_SCARLOS</t>
-  </si>
-  <si>
     <t>ZHORAY</t>
   </si>
   <si>
@@ -1171,17 +1132,56 @@
     <t>Unavailable</t>
   </si>
   <si>
-    <t>#b33c00</t>
-  </si>
-  <si>
     <t>#2bc353</t>
+  </si>
+  <si>
+    <t>CENTRAL CALOPE</t>
+  </si>
+  <si>
+    <t>CENTRAL GENEROCA</t>
+  </si>
+  <si>
+    <t>CENTRAL GASGREEN</t>
+  </si>
+  <si>
+    <t>UNACEM (CEMENTERA)</t>
+  </si>
+  <si>
+    <t>CUENCA (BAHIAS YANACOCHA GUALACEO)</t>
+  </si>
+  <si>
+    <t>LOJA 1</t>
+  </si>
+  <si>
+    <t>LOJA 2</t>
+  </si>
+  <si>
+    <t>POMASQUI A</t>
+  </si>
+  <si>
+    <t>POMASQUI B</t>
+  </si>
+  <si>
+    <t>SANTO DOMINGO A</t>
+  </si>
+  <si>
+    <t>SANTO DOMINGO B</t>
+  </si>
+  <si>
+    <t>SANTO DOMINGO C</t>
+  </si>
+  <si>
+    <t>SANTO DOMINGO</t>
+  </si>
+  <si>
+    <t>#ff0000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1210,6 +1210,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1226,13 +1232,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB33C00"/>
+        <fgColor rgb="FF2BC253"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2BC253"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1264,7 +1270,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1274,6 +1280,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF4D4D"/>
       <color rgb="FF2BC253"/>
       <color rgb="FFB33C00"/>
       <color rgb="FF00E673"/>
@@ -1558,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1589,7 @@
         <v>158</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>135</v>
@@ -1597,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>3</v>
@@ -1630,10 +1637,10 @@
         <v>'UTR_ADELCA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="1">
@@ -1652,7 +1659,7 @@
         <v>138</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -1662,10 +1669,10 @@
         <v>'UTR_AMBATO_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="1">
@@ -1684,7 +1691,7 @@
         <v>137</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>7</v>
@@ -1694,10 +1701,10 @@
         <v>'UTR_BABA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="1">
@@ -1716,7 +1723,7 @@
         <v>137</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
@@ -1726,10 +1733,10 @@
         <v>'UTR_BANOS_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="1">
@@ -1748,7 +1755,7 @@
         <v>137</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -1758,10 +1765,10 @@
         <v>'UTR_BOMBOIZA_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="1">
@@ -1780,7 +1787,7 @@
         <v>139</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
@@ -1790,10 +1797,10 @@
         <v>'UTR_C_ABANIC_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="1">
@@ -1812,7 +1819,7 @@
         <v>138</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -1822,10 +1829,10 @@
         <v>'UTR_C_AGOYAN_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="1">
@@ -1844,7 +1851,7 @@
         <v>140</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -1854,10 +1861,10 @@
         <v>'UTR_C_ALAO_D_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="1">
@@ -1876,7 +1883,7 @@
         <v>137</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -1886,10 +1893,10 @@
         <v>'UTR_C_ALAZAN_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="1">
@@ -1908,7 +1915,7 @@
         <v>141</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>14</v>
@@ -1918,10 +1925,10 @@
         <v>'UTR_C_AMBI_D_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="1">
@@ -1940,7 +1947,7 @@
         <v>137</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>15</v>
@@ -1950,10 +1957,10 @@
         <v>'UTR_C_BABA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="1">
@@ -1972,7 +1979,7 @@
         <v>139</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>170</v>
+        <v>368</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
@@ -1982,10 +1989,10 @@
         <v>'UTR_C_CALOPE_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="1">
@@ -2004,7 +2011,7 @@
         <v>137</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>17</v>
@@ -2014,10 +2021,10 @@
         <v>'UTR_C_COCACS_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="1">
@@ -2036,7 +2043,7 @@
         <v>137</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
@@ -2046,10 +2053,10 @@
         <v>'UTR_C_COCACS_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="1">
@@ -2068,7 +2075,7 @@
         <v>142</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>19</v>
@@ -2078,10 +2085,10 @@
         <v>'UTR_C_CUMBAY_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="1">
@@ -2100,7 +2107,7 @@
         <v>137</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>20</v>
@@ -2110,10 +2117,10 @@
         <v>'UTR_C_DELSIT_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="1">
@@ -2132,7 +2139,7 @@
         <v>139</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>21</v>
@@ -2142,10 +2149,10 @@
         <v>'UTR_C_DUE_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="1">
@@ -2164,7 +2171,7 @@
         <v>143</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
@@ -2174,10 +2181,10 @@
         <v>'UTR_C_ECOE_D_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="1">
@@ -2196,7 +2203,7 @@
         <v>144</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>23</v>
@@ -2206,10 +2213,10 @@
         <v>'UTR_C_ECUDOS_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="1">
@@ -2228,7 +2235,7 @@
         <v>145</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>24</v>
@@ -2238,10 +2245,10 @@
         <v>'UTR_C_ELECTR_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="1">
@@ -2260,7 +2267,7 @@
         <v>137</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>25</v>
@@ -2270,10 +2277,10 @@
         <v>'UTR_C_ESMER2_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="1">
@@ -2292,7 +2299,7 @@
         <v>142</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>26</v>
@@ -2302,10 +2309,10 @@
         <v>'UTR_C_G_HERN_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="1">
@@ -2324,7 +2331,7 @@
         <v>138</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>27</v>
@@ -2334,10 +2341,10 @@
         <v>'UTR_C_G_ZEVA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="1">
@@ -2356,7 +2363,7 @@
         <v>146</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>312</v>
+        <v>370</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>28</v>
@@ -2366,10 +2373,10 @@
         <v>'UTR_C_GASGRE_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="1">
@@ -2388,7 +2395,7 @@
         <v>157</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>309</v>
+        <v>369</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>29</v>
@@ -2398,10 +2405,10 @@
         <v>'UTR_C_GENERO_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="1">
@@ -2420,7 +2427,7 @@
         <v>142</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>30</v>
@@ -2430,10 +2437,10 @@
         <v>'UTR_C_GUAN_D_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="1">
@@ -2452,7 +2459,7 @@
         <v>137</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>31</v>
@@ -2462,10 +2469,10 @@
         <v>'UTR_C_JIVIN3_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="1">
@@ -2484,7 +2491,7 @@
         <v>147</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>147</v>
+        <v>371</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>32</v>
@@ -2494,10 +2501,10 @@
         <v>'UTR_C_LAFARG_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="1">
@@ -2516,7 +2523,7 @@
         <v>137</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>33</v>
@@ -2526,10 +2533,10 @@
         <v>'UTR_C_MANDUR_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="1">
@@ -2548,7 +2555,7 @@
         <v>137</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>34</v>
@@ -2558,10 +2565,10 @@
         <v>'UTR_C_MAZAR_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="1">
@@ -2580,7 +2587,7 @@
         <v>137</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>35</v>
@@ -2590,10 +2597,10 @@
         <v>'UTR_C_MINASF_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="1">
@@ -2612,7 +2619,7 @@
         <v>142</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>36</v>
@@ -2622,10 +2629,10 @@
         <v>'UTR_C_NAYON_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="1">
@@ -2644,7 +2651,7 @@
         <v>139</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>37</v>
@@ -2654,10 +2661,10 @@
         <v>'UTR_C_NORMAN_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="1">
@@ -2676,7 +2683,7 @@
         <v>148</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>38</v>
@@ -2686,10 +2693,10 @@
         <v>'UTR_C_PALMIR_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="1">
@@ -2708,7 +2715,7 @@
         <v>137</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>39</v>
@@ -2718,10 +2725,10 @@
         <v>'UTR_C_PASCUA_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="1">
@@ -2740,7 +2747,7 @@
         <v>138</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>40</v>
@@ -2750,10 +2757,10 @@
         <v>'UTR_C_PUCARA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="1">
@@ -2772,7 +2779,7 @@
         <v>149</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>41</v>
@@ -2782,10 +2789,10 @@
         <v>'UTR_C_PUSUN1_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="1">
@@ -2804,7 +2811,7 @@
         <v>149</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>42</v>
@@ -2814,10 +2821,10 @@
         <v>'UTR_C_PUSUN2_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="1">
@@ -2836,7 +2843,7 @@
         <v>137</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>43</v>
@@ -2846,10 +2853,10 @@
         <v>'UTR_C_QUEVE2_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="1">
@@ -2868,7 +2875,7 @@
         <v>150</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>44</v>
@@ -2878,10 +2885,10 @@
         <v>'UTR_C_RVCHIC_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="1">
@@ -2900,7 +2907,7 @@
         <v>151</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>45</v>
@@ -2910,10 +2917,10 @@
         <v>'UTR_C_S_BART_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="1">
@@ -2932,7 +2939,7 @@
         <v>152</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>46</v>
@@ -2942,10 +2949,10 @@
         <v>'UTR_C_S_CARL_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="1">
@@ -2964,7 +2971,7 @@
         <v>137</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>47</v>
@@ -2974,10 +2981,10 @@
         <v>'UTR_C_S_ELE2_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I44" s="3"/>
       <c r="J44" s="1">
@@ -2996,7 +3003,7 @@
         <v>137</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>48</v>
@@ -3006,10 +3013,10 @@
         <v>'UTR_C_S_ELE3_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="1">
@@ -3028,7 +3035,7 @@
         <v>137</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>49</v>
@@ -3038,10 +3045,10 @@
         <v>'UTR_C_S_FRAN_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="1">
@@ -3057,7 +3064,7 @@
         <v>138</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>162</v>
@@ -3067,10 +3074,10 @@
         <v>'UTR_C_S_ROSA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="1">
@@ -3086,7 +3093,7 @@
         <v>152</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>313</v>
+        <v>222</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>163</v>
@@ -3096,10 +3103,10 @@
         <v>'UTR_C_SCAR_D_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="1">
@@ -3115,10 +3122,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>50</v>
@@ -3128,10 +3135,10 @@
         <v>'UTR_C_SIBIMB_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="1">
@@ -3147,10 +3154,10 @@
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>51</v>
@@ -3160,10 +3167,10 @@
         <v>'UTR_C_SIGCHO_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="1">
@@ -3182,7 +3189,7 @@
         <v>137</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>52</v>
@@ -3192,10 +3199,10 @@
         <v>'UTR_C_SOPLAD_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="1">
@@ -3211,7 +3218,7 @@
         <v>137</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>53</v>
@@ -3221,10 +3228,10 @@
         <v>'UTR_C_T_GUAY_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="1">
@@ -3243,7 +3250,7 @@
         <v>153</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>54</v>
@@ -3253,10 +3260,10 @@
         <v>'UTR_C_TAMBO_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="1">
@@ -3272,10 +3279,10 @@
         <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>55</v>
@@ -3285,10 +3292,10 @@
         <v>'UTR_C_TOPO_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="1">
@@ -3307,7 +3314,7 @@
         <v>138</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>56</v>
@@ -3317,10 +3324,10 @@
         <v>'UTR_C_TRINIT_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="1">
@@ -3333,10 +3340,10 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>57</v>
@@ -3346,10 +3353,10 @@
         <v>'UTR_C_VICTO2_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="1">
@@ -3365,10 +3372,10 @@
         <v>4</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>58</v>
@@ -3378,10 +3385,10 @@
         <v>'UTR_C_VICTOR_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="1">
@@ -3400,7 +3407,7 @@
         <v>137</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>59</v>
@@ -3410,10 +3417,10 @@
         <v>'UTR_C_VILLON_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="1">
@@ -3432,7 +3439,7 @@
         <v>137</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>60</v>
@@ -3442,10 +3449,10 @@
         <v>'UTR_CARAGUAY_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="1">
@@ -3464,7 +3471,7 @@
         <v>138</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>61</v>
@@ -3474,10 +3481,10 @@
         <v>'UTR_CHONE_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="1">
@@ -3496,7 +3503,7 @@
         <v>137</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>62</v>
@@ -3506,10 +3513,10 @@
         <v>'UTR_CHONGON_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="1">
@@ -3528,7 +3535,7 @@
         <v>137</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>63</v>
@@ -3538,10 +3545,10 @@
         <v>'UTR_CHORRILL_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="1">
@@ -3560,7 +3567,7 @@
         <v>137</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>164</v>
@@ -3570,10 +3577,10 @@
         <v>'UTR_CONCORDI_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="1">
@@ -3589,7 +3596,7 @@
         <v>137</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>64</v>
@@ -3599,10 +3606,10 @@
         <v>'UTR_CUENCA_1_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="1">
@@ -3621,7 +3628,7 @@
         <v>137</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>245</v>
+        <v>372</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>65</v>
@@ -3631,10 +3638,10 @@
         <v>'UTR_CUENCA_2_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="1">
@@ -3653,7 +3660,7 @@
         <v>138</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>66</v>
@@ -3663,10 +3670,10 @@
         <v>'UTR_CUENCA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I66" s="3"/>
       <c r="J66" s="1">
@@ -3685,7 +3692,7 @@
         <v>137</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>67</v>
@@ -3695,10 +3702,10 @@
         <v>'UTR_CUMBARAT_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I67" s="3"/>
       <c r="J67" s="1">
@@ -3717,7 +3724,7 @@
         <v>137</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>68</v>
@@ -3727,10 +3734,10 @@
         <v>'UTR_D_CERRIT_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I68" s="3"/>
       <c r="J68" s="1">
@@ -3746,7 +3753,7 @@
         <v>137</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>69</v>
@@ -3756,10 +3763,10 @@
         <v>'UTR_D_PERIPA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I69" s="3"/>
       <c r="J69" s="1">
@@ -3778,7 +3785,7 @@
         <v>137</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>70</v>
@@ -3788,10 +3795,10 @@
         <v>'UTR_DURAN_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I70" s="3"/>
       <c r="J70" s="1">
@@ -3810,7 +3817,7 @@
         <v>137</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>71</v>
@@ -3820,10 +3827,10 @@
         <v>'UTR_E_GUAYAQ_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I71" s="3"/>
       <c r="J71" s="1">
@@ -3842,7 +3849,7 @@
         <v>154</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>72</v>
@@ -3852,10 +3859,10 @@
         <v>'UTR_EMAP_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I72" s="3"/>
       <c r="J72" s="1">
@@ -3874,7 +3881,7 @@
         <v>137</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>73</v>
@@ -3884,10 +3891,10 @@
         <v>'UTR_ESCLUSAS_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I73" s="3"/>
       <c r="J73" s="1">
@@ -3906,7 +3913,7 @@
         <v>137</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>74</v>
@@ -3916,10 +3923,10 @@
         <v>'UTR_ESMERALD_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I74" s="3"/>
       <c r="J74" s="1">
@@ -3938,7 +3945,7 @@
         <v>138</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>75</v>
@@ -3948,10 +3955,10 @@
         <v>'UTR_ESMERALD_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="1">
@@ -3967,10 +3974,10 @@
         <v>4</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>165</v>
@@ -3980,10 +3987,10 @@
         <v>'UTR_F_NORTE _IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I76" s="3"/>
       <c r="J76" s="1">
@@ -4002,7 +4009,7 @@
         <v>137</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>76</v>
@@ -4012,10 +4019,10 @@
         <v>'UTR_GUALACEO_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I77" s="3"/>
       <c r="J77" s="1">
@@ -4034,7 +4041,7 @@
         <v>137</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>77</v>
@@ -4044,10 +4051,10 @@
         <v>'UTR_IBARRA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I78" s="3"/>
       <c r="J78" s="1">
@@ -4066,7 +4073,7 @@
         <v>155</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>78</v>
@@ -4076,10 +4083,10 @@
         <v>'UTR_INCOMING_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I79" s="3"/>
       <c r="J79" s="1">
@@ -4098,7 +4105,7 @@
         <v>137</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>79</v>
@@ -4108,10 +4115,10 @@
         <v>'UTR_INGA_500_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I80" s="3"/>
       <c r="J80" s="1">
@@ -4130,7 +4137,7 @@
         <v>137</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>80</v>
@@ -4140,10 +4147,10 @@
         <v>'UTR_INGA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I81" s="3"/>
       <c r="J81" s="1">
@@ -4162,7 +4169,7 @@
         <v>138</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>81</v>
@@ -4172,10 +4179,10 @@
         <v>'UTR_JIVINO_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I82" s="3"/>
       <c r="J82" s="1">
@@ -4194,7 +4201,7 @@
         <v>137</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>82</v>
@@ -4204,10 +4211,10 @@
         <v>'UTR_LIMON_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I83" s="3"/>
       <c r="J83" s="1">
@@ -4223,7 +4230,7 @@
         <v>137</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>261</v>
+        <v>373</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>83</v>
@@ -4233,10 +4240,10 @@
         <v>'UTR_LOJA_1_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I84" s="3"/>
       <c r="J84" s="1">
@@ -4255,7 +4262,7 @@
         <v>137</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>262</v>
+        <v>374</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>84</v>
@@ -4265,10 +4272,10 @@
         <v>'UTR_LOJA_2_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I85" s="3"/>
       <c r="J85" s="1">
@@ -4287,7 +4294,7 @@
         <v>138</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>85</v>
@@ -4297,10 +4304,10 @@
         <v>'UTR_LOJA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I86" s="3"/>
       <c r="J86" s="1">
@@ -4319,7 +4326,7 @@
         <v>137</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>86</v>
@@ -4329,10 +4336,10 @@
         <v>'UTR_LORETO_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I87" s="3"/>
       <c r="J87" s="1">
@@ -4351,7 +4358,7 @@
         <v>137</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>87</v>
@@ -4361,10 +4368,10 @@
         <v>'UTR_MACAS_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I88" s="3"/>
       <c r="J88" s="1">
@@ -4383,7 +4390,7 @@
         <v>137</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>88</v>
@@ -4393,10 +4400,10 @@
         <v>'UTR_MACHALA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I89" s="3"/>
       <c r="J89" s="1">
@@ -4415,7 +4422,7 @@
         <v>137</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>89</v>
@@ -4425,10 +4432,10 @@
         <v>'UTR_MENDEZ_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I90" s="3"/>
       <c r="J90" s="1">
@@ -4447,7 +4454,7 @@
         <v>137</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>90</v>
@@ -4457,10 +4464,10 @@
         <v>'UTR_MILAGRO_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I91" s="3"/>
       <c r="J91" s="1">
@@ -4479,7 +4486,7 @@
         <v>137</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>91</v>
@@ -4489,10 +4496,10 @@
         <v>'UTR_MIRADOR_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I92" s="3"/>
       <c r="J92" s="1">
@@ -4511,7 +4518,7 @@
         <v>138</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>92</v>
@@ -4521,10 +4528,10 @@
         <v>'UTR_MOLINO_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I93" s="3"/>
       <c r="J93" s="1">
@@ -4543,7 +4550,7 @@
         <v>138</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>93</v>
@@ -4553,10 +4560,10 @@
         <v>'UTR_MULALO_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I94" s="3"/>
       <c r="J94" s="1">
@@ -4575,7 +4582,7 @@
         <v>137</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>94</v>
@@ -4585,10 +4592,10 @@
         <v>'UTR_N_BABAHO_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I95" s="3"/>
       <c r="J95" s="1">
@@ -4607,7 +4614,7 @@
         <v>137</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>95</v>
@@ -4617,10 +4624,10 @@
         <v>'UTR_N_PROSPE_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I96" s="3"/>
       <c r="J96" s="1">
@@ -4639,7 +4646,7 @@
         <v>137</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>96</v>
@@ -4649,10 +4656,10 @@
         <v>'UTR_P_NAPO_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I97" s="3"/>
       <c r="J97" s="1">
@@ -4671,7 +4678,7 @@
         <v>137</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>97</v>
@@ -4681,10 +4688,10 @@
         <v>'UTR_PASCUALE_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I98" s="3"/>
       <c r="J98" s="1">
@@ -4713,10 +4720,10 @@
         <v>'UTR_PETROAMA_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I99" s="3"/>
       <c r="J99" s="1">
@@ -4735,7 +4742,7 @@
         <v>138</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>99</v>
@@ -4745,10 +4752,10 @@
         <v>'UTR_POLICENT_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I100" s="3"/>
       <c r="J100" s="1">
@@ -4767,7 +4774,7 @@
         <v>137</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>277</v>
+        <v>375</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>100</v>
@@ -4777,10 +4784,10 @@
         <v>'UTR_POMASQUI_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I101" s="3"/>
       <c r="J101" s="1">
@@ -4799,7 +4806,7 @@
         <v>138</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>278</v>
+        <v>376</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>101</v>
@@ -4809,10 +4816,10 @@
         <v>'UTR_POMASQUI_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I102" s="3"/>
       <c r="J102" s="1">
@@ -4831,7 +4838,7 @@
         <v>138</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>102</v>
@@ -4841,10 +4848,10 @@
         <v>'UTR_PORTOVIE_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I103" s="3"/>
       <c r="J103" s="1">
@@ -4863,7 +4870,7 @@
         <v>138</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>103</v>
@@ -4873,10 +4880,10 @@
         <v>'UTR_POSORJA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I104" s="3"/>
       <c r="J104" s="1">
@@ -4895,7 +4902,7 @@
         <v>137</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>104</v>
@@ -4905,10 +4912,10 @@
         <v>'UTR_QUEVEDO_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I105" s="3"/>
       <c r="J105" s="1">
@@ -4927,7 +4934,7 @@
         <v>137</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>105</v>
@@ -4937,10 +4944,10 @@
         <v>'UTR_QUININDE_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I106" s="3"/>
       <c r="J106" s="1">
@@ -4959,7 +4966,7 @@
         <v>138</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>106</v>
@@ -4969,10 +4976,10 @@
         <v>'UTR_RIOBAMBA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I107" s="3"/>
       <c r="J107" s="1">
@@ -4991,7 +4998,7 @@
         <v>137</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>284</v>
+        <v>377</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>107</v>
@@ -5001,10 +5008,10 @@
         <v>'UTR_S_DOMI_2_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I108" s="3"/>
       <c r="J108" s="1">
@@ -5023,7 +5030,7 @@
         <v>137</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>285</v>
+        <v>378</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>108</v>
@@ -5033,10 +5040,10 @@
         <v>'UTR_S_DOMING_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I109" s="3"/>
       <c r="J109" s="1">
@@ -5055,7 +5062,7 @@
         <v>137</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>286</v>
+        <v>379</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>109</v>
@@ -5065,10 +5072,10 @@
         <v>'UTR_S_DOMING_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I110" s="3"/>
       <c r="J110" s="1">
@@ -5084,7 +5091,7 @@
         <v>137</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>171</v>
+        <v>380</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>110</v>
@@ -5094,10 +5101,10 @@
         <v>'UTR_S_DOMING_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I111" s="3"/>
       <c r="J111" s="1">
@@ -5116,7 +5123,7 @@
         <v>137</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>111</v>
@@ -5126,10 +5133,10 @@
         <v>'UTR_S_ELENA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I112" s="3"/>
       <c r="J112" s="1">
@@ -5148,7 +5155,7 @@
         <v>138</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>112</v>
@@ -5158,10 +5165,10 @@
         <v>'UTR_S_ELENA_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I113" s="3"/>
       <c r="J113" s="1">
@@ -5180,7 +5187,7 @@
         <v>137</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>113</v>
@@ -5190,10 +5197,10 @@
         <v>'UTR_S_GREGOR_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I114" s="3"/>
       <c r="J114" s="1">
@@ -5212,7 +5219,7 @@
         <v>137</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>114</v>
@@ -5222,10 +5229,10 @@
         <v>'UTR_S_IDELFO_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I115" s="3"/>
       <c r="J115" s="1">
@@ -5244,7 +5251,7 @@
         <v>137</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>115</v>
@@ -5254,10 +5261,10 @@
         <v>'UTR_S_RAFAEL_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I116" s="3"/>
       <c r="J116" s="1">
@@ -5276,7 +5283,7 @@
         <v>137</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>116</v>
@@ -5286,10 +5293,10 @@
         <v>'UTR_S_ROSA_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H117" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I117" s="3"/>
       <c r="J117" s="1">
@@ -5308,7 +5315,7 @@
         <v>137</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>117</v>
@@ -5318,10 +5325,10 @@
         <v>'UTR_SALITRAL_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I118" s="3"/>
       <c r="J118" s="1">
@@ -5340,7 +5347,7 @@
         <v>137</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>118</v>
@@ -5350,10 +5357,10 @@
         <v>'UTR_SHUSHUFI_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I119" s="3"/>
       <c r="J119" s="1">
@@ -5372,7 +5379,7 @@
         <v>137</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>119</v>
@@ -5382,10 +5389,10 @@
         <v>'UTR_SININCAY_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I120" s="3"/>
       <c r="J120" s="1">
@@ -5401,7 +5408,7 @@
         <v>138</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>120</v>
@@ -5411,10 +5418,10 @@
         <v>'UTR_SURVALEN_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I121" s="3"/>
       <c r="J121" s="1">
@@ -5433,7 +5440,7 @@
         <v>137</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>121</v>
@@ -5443,10 +5450,10 @@
         <v>'UTR_TADAY_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I122" s="3"/>
       <c r="J122" s="1">
@@ -5462,7 +5469,7 @@
         <v>138</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>166</v>
@@ -5472,10 +5479,10 @@
         <v>'UTR_TBOX_DNP30TCPIP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I123" s="3"/>
       <c r="J123" s="1">
@@ -5494,7 +5501,7 @@
         <v>137</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>122</v>
@@ -5504,10 +5511,10 @@
         <v>'UTR_TERMOESM_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I124" s="3"/>
       <c r="J124" s="1">
@@ -5526,7 +5533,7 @@
         <v>161</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>123</v>
@@ -5536,10 +5543,10 @@
         <v>'UTR_TERMOPIC_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I125" s="3"/>
       <c r="J125" s="1">
@@ -5555,7 +5562,7 @@
         <v>138</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>167</v>
@@ -5565,10 +5572,10 @@
         <v>'UTR_TEST_LAB_DNP.SV'="DISPONIBLE"</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I126" s="3"/>
       <c r="J126" s="1">
@@ -5584,7 +5591,7 @@
         <v>138</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>168</v>
@@ -5594,10 +5601,10 @@
         <v>'UTR_TEST_LAB_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I127" s="3"/>
       <c r="J127" s="1">
@@ -5614,7 +5621,7 @@
         <v>138</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E128" s="7" t="s">
         <v>169</v>
@@ -5624,10 +5631,10 @@
         <v>'UTR_TEST_LAB_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I128" s="3"/>
       <c r="J128" s="1">
@@ -5646,7 +5653,7 @@
         <v>137</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>124</v>
@@ -5656,10 +5663,10 @@
         <v>'UTR_TGMA_COR_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I129" s="3"/>
       <c r="J129" s="1">
@@ -5678,7 +5685,7 @@
         <v>137</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>125</v>
@@ -5688,10 +5695,10 @@
         <v>'UTR_TISALEO_IEC8705104.SV'="DISPONIBLE"</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I130" s="3"/>
       <c r="J130" s="1">
@@ -5710,7 +5717,7 @@
         <v>137</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>126</v>
@@ -5720,10 +5727,10 @@
         <v>'UTR_TOPO_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I131" s="3"/>
       <c r="J131" s="1">
@@ -5742,7 +5749,7 @@
         <v>137</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>127</v>
@@ -5752,10 +5759,10 @@
         <v>'UTR_TOTORAS_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I132" s="3"/>
       <c r="J132" s="1">
@@ -5774,7 +5781,7 @@
         <v>138</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>128</v>
@@ -5784,10 +5791,10 @@
         <v>'UTR_TOTORAS_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I133" s="3"/>
       <c r="J133" s="1">
@@ -5806,7 +5813,7 @@
         <v>138</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>129</v>
@@ -5816,10 +5823,10 @@
         <v>'UTR_TRINITAR_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I134" s="3"/>
       <c r="J134" s="1">
@@ -5838,7 +5845,7 @@
         <v>138</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>130</v>
@@ -5848,10 +5855,10 @@
         <v>'UTR_TULCAN_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I135" s="3"/>
       <c r="J135" s="1">
@@ -5867,7 +5874,7 @@
         <v>138</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>131</v>
@@ -5877,10 +5884,10 @@
         <v>'UTR_VICENTIN_RP5.SV'="DISPONIBLE"</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="1">
@@ -5899,7 +5906,7 @@
         <v>137</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>132</v>
@@ -5909,10 +5916,10 @@
         <v>'UTR_VILLONAC_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="1">
@@ -5931,7 +5938,7 @@
         <v>137</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>133</v>
@@ -5941,10 +5948,10 @@
         <v>'UTR_YANACOCH_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="1">
@@ -5963,7 +5970,7 @@
         <v>137</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>134</v>
@@ -5973,10 +5980,10 @@
         <v>'UTR_ZHORAY_IEC8705101.SV'="DISPONIBLE"</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I139" s="3"/>
       <c r="J139" s="1">
@@ -6016,7 +6023,7 @@
         <v>158</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>4</v>
@@ -6028,7 +6035,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>2</v>
@@ -6037,7 +6044,7 @@
         <v>156</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6048,17 +6055,17 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="E2" s="3" t="str">
         <f>CONCATENATE("'",D2,"'","=","""Up""")</f>
         <v>'ICCP_CND_STATUS.SV'="Up"</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -6070,17 +6077,17 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" ref="E3:E13" si="0">CONCATENATE("'",D3,"'","=","""Up""")</f>
         <v>'ICCP_TRN_STATUS.SV'="Up"</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -6092,17 +6099,17 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_CCGHP_STATUS.SV'="Up"</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -6114,17 +6121,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_SIGDE_STATUS.SV'="Up"</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -6136,17 +6143,17 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_EAUT_STATUS.SV'="Up"</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -6158,17 +6165,17 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_JARM_STATUS.SV'="Up"</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -6180,17 +6187,17 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="E8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_EGYQ_STATUS.SV'="Up"</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -6202,17 +6209,17 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_TGMA_STATUS.SV'="Up"</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G9" s="3"/>
     </row>
@@ -6224,17 +6231,17 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_SDOM_STATUS.SV'="Up"</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G10" s="3"/>
     </row>
@@ -6246,17 +6253,17 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_SPS_STATUS.SV'="Up"</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -6268,17 +6275,17 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_ERS_STATUS.SV'="Up"</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -6290,17 +6297,17 @@
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>'ICCP_DPE_STATUS.SV'="Up"</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -6963,7 +6970,7 @@
         <v>158</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>4</v>
@@ -6975,7 +6982,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6986,10 +6993,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="E2" s="3" t="str">
         <f>CONCATENATE("'",D2,"'","=","""GRUPO""")</f>
@@ -7436,95 +7443,95 @@
   <sheetData>
     <row r="1" spans="2:7" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B1" s="11" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -7537,7 +7544,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7547,30 +7554,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>381</v>
+        <v>360</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>368</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>380</v>
+        <v>355</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7589,58 +7597,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="B2" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="B3" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="B5" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="B6" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reporte automático de SSAA - inclusión de la matriz de riesgo
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sRemoto" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="410">
   <si>
     <t>Tag</t>
   </si>
@@ -1694,7 +1694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J139"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6284,14 +6286,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6316,9 +6318,6 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>159</v>
-      </c>
       <c r="B2" t="s">
         <v>393</v>
       </c>

</xml_diff>